<commit_message>
Update sample data file with complete 15-shipment dataset
</commit_message>
<xml_diff>
--- a/Sample_Data.xlsx
+++ b/Sample_Data.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shipments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Shipment ID</t>
+          <t>Unique identifier</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Collection Location</t>
+          <t>Collection Area Name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Delivery Location</t>
+          <t>Delivery Area Name</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -471,17 +471,27 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Carrier</t>
+          <t>Shipper</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Weight (kg)</t>
+          <t>Emission type by shipper mode</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Cost</t>
+          <t>Emission factor of emission type</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Cost of shipment</t>
         </is>
       </c>
     </row>
@@ -526,10 +536,18 @@
           <t>DPD</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="K2" t="n">
         <v>5.5</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -574,10 +592,18 @@
           <t>Royal Mail</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="K3" t="n">
         <v>12</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>25</v>
       </c>
     </row>
@@ -622,10 +648,18 @@
           <t>DHL Express</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Air Freight</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K4" t="n">
         <v>8</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>85</v>
       </c>
     </row>
@@ -670,10 +704,18 @@
           <t>FedEx</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="K5" t="n">
         <v>25</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
         <v>45</v>
       </c>
     </row>
@@ -718,10 +760,18 @@
           <t>UPS</t>
         </is>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Air Freight</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="K6" t="n">
         <v>15</v>
       </c>
-      <c r="J6" t="n">
+      <c r="L6" t="n">
         <v>95</v>
       </c>
     </row>
@@ -766,10 +816,18 @@
           <t>ParcelForce</t>
         </is>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="K7" t="n">
         <v>3.5</v>
       </c>
-      <c r="J7" t="n">
+      <c r="L7" t="n">
         <v>8.5</v>
       </c>
     </row>
@@ -814,10 +872,18 @@
           <t>Maersk</t>
         </is>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Container Ship</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="K8" t="n">
         <v>500</v>
       </c>
-      <c r="J8" t="n">
+      <c r="L8" t="n">
         <v>250</v>
       </c>
     </row>
@@ -862,10 +928,18 @@
           <t>DHL</t>
         </is>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="K9" t="n">
         <v>18</v>
       </c>
-      <c r="J9" t="n">
+      <c r="L9" t="n">
         <v>55</v>
       </c>
     </row>
@@ -910,10 +984,18 @@
           <t>Iberia Cargo</t>
         </is>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Air Freight</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="K10" t="n">
         <v>10</v>
       </c>
-      <c r="J10" t="n">
+      <c r="L10" t="n">
         <v>78</v>
       </c>
     </row>
@@ -958,11 +1040,299 @@
           <t>Hermes</t>
         </is>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K11" t="n">
         <v>6</v>
       </c>
-      <c r="J11" t="n">
+      <c r="L11" t="n">
         <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SHIP011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2024-11-11</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Road</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Australia Post</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K12" t="n">
+        <v>20</v>
+      </c>
+      <c r="L12" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SHIP012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2024-11-12</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>W1A 1AA</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>100-0001</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Air</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>FedEx</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Air Freight</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K13" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="L13" t="n">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SHIP013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2024-11-13</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>OX1 2JD</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>CB2 1TN</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Road</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>DPD</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="K14" t="n">
+        <v>4</v>
+      </c>
+      <c r="L14" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SHIP014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2024-11-14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>75001</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>00100</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Road</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>TNT</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="K15" t="n">
+        <v>30</v>
+      </c>
+      <c r="L15" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SHIP015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2024-11-15</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CR0 1EA</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>BN1 1AL</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Road</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Royal Mail</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Van</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="K16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L16" t="n">
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>